<commit_message>
Add data for stacked chart
</commit_message>
<xml_diff>
--- a/data/data/USDetail/select_msn/sankey/sankey.xlsx
+++ b/data/data/USDetail/select_msn/sankey/sankey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\An\Documents\GitHub\COS30045\data\data\USDetail\select_msn\sankey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA460D7-9F05-4DA0-B4B7-C270BCAE1927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3088DA-3777-4B91-A5EB-3E17A080CD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="24" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="213">
   <si>
     <t>MSN</t>
   </si>
@@ -678,6 +678,12 @@
   </si>
   <si>
     <t>Total energy consumption</t>
+  </si>
+  <si>
+    <t>Total consumption</t>
+  </si>
+  <si>
+    <t>Consumption</t>
   </si>
 </sst>
 </file>
@@ -1551,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD520A74-6D21-4711-8177-C48F7CF78287}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3664,9 +3670,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E865CF0B-C2EB-4915-A8EA-926F7C386763}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3809,6 +3817,17 @@
         <v>38</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3816,9 +3835,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DF2398-0B2C-439E-B3E0-5AB695475E69}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4033,6 +4054,46 @@
         <v>189</v>
       </c>
     </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>212</v>
+      </c>
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>212</v>
+      </c>
+      <c r="B28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>212</v>
+      </c>
+      <c r="B29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>212</v>
+      </c>
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>212</v>
+      </c>
+      <c r="B31" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>